<commit_message>
feat: finished tracking down which variables feed into the end FIM result
I've now fully tracked which outputs get created in which steps of FIM calculation, and recorded them in the spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/variables_tracker.xlsx
+++ b/docs/variables_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\FIM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD710EB5-C5B8-4C04-AFC2-071A0FF46078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB5A16A-0506-4535-B320-86CFB0B9F284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="115">
   <si>
     <t>Step 1: Input</t>
   </si>
@@ -232,13 +232,151 @@
   </si>
   <si>
     <t>Step 5: Calculate contribution</t>
+  </si>
+  <si>
+    <t>Step 6: Sum contribution</t>
+  </si>
+  <si>
+    <t>These variables are calculated in section E: Contribution</t>
+  </si>
+  <si>
+    <t>federal_purchases_contribution</t>
+  </si>
+  <si>
+    <t>state_purchases_contribution</t>
+  </si>
+  <si>
+    <t>federal_subsidies_contribution</t>
+  </si>
+  <si>
+    <t>federal_aid_to_small_businesses_arp_contribution</t>
+  </si>
+  <si>
+    <t>federal_ui_contribution</t>
+  </si>
+  <si>
+    <t>state_ui_contribution</t>
+  </si>
+  <si>
+    <t>rebate_checks_contribution</t>
+  </si>
+  <si>
+    <t>rebate_checks_arp_contribution</t>
+  </si>
+  <si>
+    <t>federal_other_vulnerable_arp_contribution</t>
+  </si>
+  <si>
+    <t>federal_other_direct_aid_arp_contribution</t>
+  </si>
+  <si>
+    <t>federal_social_benefits_contribution</t>
+  </si>
+  <si>
+    <t>state_social_benefits_contribution</t>
+  </si>
+  <si>
+    <t>federal_non_corporate_taxes_contribution</t>
+  </si>
+  <si>
+    <t>state_non_corporate_taxes_contribution</t>
+  </si>
+  <si>
+    <t>federal_corporate_taxes_contribution</t>
+  </si>
+  <si>
+    <t>state_corporate_taxes_contribution</t>
+  </si>
+  <si>
+    <t>federal_student_loans_contribution</t>
+  </si>
+  <si>
+    <t>supply_side_ira_contribution</t>
+  </si>
+  <si>
+    <t>consumption_grants_contribution</t>
+  </si>
+  <si>
+    <t>investment_grants_contribution</t>
+  </si>
+  <si>
+    <t>social_benefits_contribution</t>
+  </si>
+  <si>
+    <t>corporate_taxes_contribution</t>
+  </si>
+  <si>
+    <t>non_corporate_taxes_contribution</t>
+  </si>
+  <si>
+    <t>subsidies_contribution</t>
+  </si>
+  <si>
+    <t>state_subsidies_contribution</t>
+  </si>
+  <si>
+    <t>health_outlays_contribution</t>
+  </si>
+  <si>
+    <t>federal_health_outlays_contribution</t>
+  </si>
+  <si>
+    <t>state_health_outlays_contribution</t>
+  </si>
+  <si>
+    <t>grants_contribution</t>
+  </si>
+  <si>
+    <t>federal_contribution</t>
+  </si>
+  <si>
+    <t>state_contribution</t>
+  </si>
+  <si>
+    <t>overwrites already calculated</t>
+  </si>
+  <si>
+    <t>overwrites and uses already calculated</t>
+  </si>
+  <si>
+    <t>taxes_contribution</t>
+  </si>
+  <si>
+    <t>warning: does not include supply side ira</t>
+  </si>
+  <si>
+    <t>unless corporate taxes contribution does</t>
+  </si>
+  <si>
+    <t>transfers_contribution</t>
+  </si>
+  <si>
+    <t>calculated again</t>
+  </si>
+  <si>
+    <t>Step 7 Get Fiscal Impact</t>
+  </si>
+  <si>
+    <t>this is in the get_fiscal_impact function</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>What we input:</t>
+  </si>
+  <si>
+    <t>&lt;- we're missing these from the inputs</t>
+  </si>
+  <si>
+    <t>&lt;- we're missing these from the outputs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,16 +390,57 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF6600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -269,22 +448,118 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -559,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="53" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,9 +847,14 @@
     <col min="3" max="3" width="31.81640625" customWidth="1"/>
     <col min="4" max="4" width="29.81640625" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" customWidth="1"/>
+    <col min="7" max="7" width="42.7265625" customWidth="1"/>
+    <col min="8" max="8" width="34.1796875" customWidth="1"/>
+    <col min="9" max="9" width="43.6328125" customWidth="1"/>
+    <col min="11" max="11" width="31.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,8 +870,14 @@
       <c r="E1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -601,40 +887,113 @@
       <c r="C2" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -647,8 +1006,19 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -661,8 +1031,21 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -675,8 +1058,24 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -689,32 +1088,87 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -727,8 +1181,26 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -741,8 +1213,24 @@
       <c r="D15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -755,8 +1243,24 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -769,8 +1273,24 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -783,8 +1303,24 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -797,8 +1333,24 @@
       <c r="D19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -808,8 +1360,24 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -819,8 +1387,22 @@
       <c r="D21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -833,8 +1415,29 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="O22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -847,8 +1450,26 @@
       <c r="D23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -861,8 +1482,26 @@
       <c r="D24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -875,8 +1514,22 @@
       <c r="D25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
@@ -886,8 +1539,22 @@
       <c r="D26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="K26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
@@ -897,8 +1564,22 @@
       <c r="D27" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>45</v>
       </c>
@@ -908,8 +1589,15 @@
       <c r="D28" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>46</v>
       </c>
@@ -919,8 +1607,21 @@
       <c r="D29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>47</v>
       </c>
@@ -930,8 +1631,18 @@
       <c r="D30" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>48</v>
       </c>
@@ -941,8 +1652,18 @@
       <c r="D31" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>49</v>
       </c>
@@ -952,8 +1673,15 @@
       <c r="D32" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="E32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>50</v>
       </c>
@@ -963,11 +1691,115 @@
       <c r="D33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="E33" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>52</v>
       </c>
+      <c r="F34" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F35" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F36" s="8"/>
+      <c r="G36" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F37" s="8"/>
+      <c r="G37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F38" s="10"/>
+      <c r="G38" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F39" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F40" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F41" s="4"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F42" s="4"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F43" s="4"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F44" s="4"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F45" s="4"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F46" s="4"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F47" s="4"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F48" s="4"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F49" s="4"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F50" s="4"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F51" s="4"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G52" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
docs: create pipeline diagram for how FIM inputs lead to FIM outputs
I've finally cracked the FIM! Well, at least the calculation steps. (There's still a lot of work to be done to understand how our data is gathered into a data frame for use in the FIM). Still, this Excel sheet now shows how the 24 variables in the forecast sheet lead to the 4 FIM output variables in very clear detail. With this done, I'm now prepared to refactor the entire calculations section.
</commit_message>
<xml_diff>
--- a/docs/variables_tracker.xlsx
+++ b/docs/variables_tracker.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\FIM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB5A16A-0506-4535-B320-86CFB0B9F284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD810A0-43DE-4347-B4A6-8669173481BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-3390" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="3" r:id="rId1"/>
+    <sheet name="map series to analysis" sheetId="1" r:id="rId2"/>
+    <sheet name="FIM summary Jun24" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="240">
   <si>
     <t>Step 1: Input</t>
   </si>
@@ -370,13 +372,388 @@
   </si>
   <si>
     <t>&lt;- we're missing these from the outputs</t>
+  </si>
+  <si>
+    <t>How we calculate the FIM</t>
+  </si>
+  <si>
+    <t>federal purchases</t>
+  </si>
+  <si>
+    <t>input (x)</t>
+  </si>
+  <si>
+    <t>y = 400 * (x - lag(x) * (1 + fed purch defl g + rpgg))/lag(gdp)</t>
+  </si>
+  <si>
+    <t>federal purchases contribution</t>
+  </si>
+  <si>
+    <t>state purchases</t>
+  </si>
+  <si>
+    <t>y = 400 * (x - lag(x) * (1 + state purch defl g + rpgg))/lag(gdp)</t>
+  </si>
+  <si>
+    <t>state purchases contribution</t>
+  </si>
+  <si>
+    <t>consumption grants</t>
+  </si>
+  <si>
+    <t>investment grants</t>
+  </si>
+  <si>
+    <t>y = 400 * (x - lag(x) * (1 + cons gr defl g + rpgg))/lag(gdp)</t>
+  </si>
+  <si>
+    <t>y = 400 * (x - lag(x) * (1 + inv gr defl g + rpgg))/lag(gdp)</t>
+  </si>
+  <si>
+    <t>consumption grants contribution</t>
+  </si>
+  <si>
+    <t>investment grants contribution</t>
+  </si>
+  <si>
+    <t>federal contribution</t>
+  </si>
+  <si>
+    <t>state contribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z = federal purchases contribution + consumption grants contribution + investment grants contribution </t>
+  </si>
+  <si>
+    <t>z = state purchases contribution - consumption grants contribution - investment grants contribution</t>
+  </si>
+  <si>
+    <t>taxes contribution</t>
+  </si>
+  <si>
+    <t>"minus neutral" throughput (a)</t>
+  </si>
+  <si>
+    <t>a = x - lag(x) * (1 + rpgg +cdg)</t>
+  </si>
+  <si>
+    <t>federal non corporate taxes minus neutral</t>
+  </si>
+  <si>
+    <t>state non corporate taxes minus neutral</t>
+  </si>
+  <si>
+    <t>federal corporate taxes minus neutral</t>
+  </si>
+  <si>
+    <t>supply side ira minus neutral</t>
+  </si>
+  <si>
+    <t>state corporate taxes minus neutral</t>
+  </si>
+  <si>
+    <t>$mpc06 [1] -0.12 -0.12 -0.06 -0.06 -0.06 -0.06 -0.06 -0.06</t>
+  </si>
+  <si>
+    <t>$mpc05  [1] -0.03333 -0.03333 -0.03333 -0.03333 -0.03333 -0.03333 -0.03333 -0.03333 -0.03333 -0.03333 -0.03333  -0.03333</t>
+  </si>
+  <si>
+    <t>$mpc_direct [1] 1</t>
+  </si>
+  <si>
+    <t>"post mpc" throughput (b)</t>
+  </si>
+  <si>
+    <t>federal non corporate taxes post mpc</t>
+  </si>
+  <si>
+    <t>state non corporate taxes post mpc</t>
+  </si>
+  <si>
+    <t>federal corporate taxes post mpc</t>
+  </si>
+  <si>
+    <t>supply side ira post mpc</t>
+  </si>
+  <si>
+    <t>state corporate taxes post mpc</t>
+  </si>
+  <si>
+    <t>y = 400*b / lag(gdp)</t>
+  </si>
+  <si>
+    <t>federal non corporate taxes contribution</t>
+  </si>
+  <si>
+    <t>state non corporate taxes contribution</t>
+  </si>
+  <si>
+    <t>federal corporate taxes contribution</t>
+  </si>
+  <si>
+    <t>supply side ira contribution</t>
+  </si>
+  <si>
+    <t>state corporate taxes contribution</t>
+  </si>
+  <si>
+    <t>z = federal non corporate taxes contribution + state non corporate taxes contribution + federal corporate taxes contribution + supply side ira contribution + state corporate taxes contribution</t>
+  </si>
+  <si>
+    <t>transfers contribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z = federal_social_benefits_contribution + state social benefits contribution + rebate checks contribution + rebate checks arp contribution + federal ui contribution + state ui contribution + federal subsidies contribution + federal aid to small businesses arp contribution  + federal otehr direct aid arp contribution + federal other vulnerable arp contribution + federal student loans contribution + state subsidies contribution + federal health outlays contribution +  state health outlays contribution </t>
+  </si>
+  <si>
+    <t>state subsidies minus neutral</t>
+  </si>
+  <si>
+    <t>federal health outlays minus neutral</t>
+  </si>
+  <si>
+    <t>state health outlays minus neutral</t>
+  </si>
+  <si>
+    <t>$mpc03 [1] 0.04950 0.04275 0.04050 0.03825 0.03375 0.03375 0.03375 0.03375 0.02700 0.02700 0.02700 0.02700 0.00900 0.00900 0.00900 0.00900</t>
+  </si>
+  <si>
+    <t>$mpc04 [1] 0.225 0.225 0.225 0.225</t>
+  </si>
+  <si>
+    <t>state subsidies post mpc</t>
+  </si>
+  <si>
+    <t>federal health outlays post mpc</t>
+  </si>
+  <si>
+    <t>state health outlays post mpc</t>
+  </si>
+  <si>
+    <t>contributions output (y)</t>
+  </si>
+  <si>
+    <t>binned contributions output (z)</t>
+  </si>
+  <si>
+    <t>federal health outlays</t>
+  </si>
+  <si>
+    <t>x = medicare + medicaid_grants</t>
+  </si>
+  <si>
+    <t>medicaid grants</t>
+  </si>
+  <si>
+    <t>state health outlays</t>
+  </si>
+  <si>
+    <t>x = medicaid - medicaid_grants</t>
+  </si>
+  <si>
+    <t>we don't have subsidies in the forecast sheet so we auto project them to equal 0</t>
+  </si>
+  <si>
+    <t>federal social benefits post mpc</t>
+  </si>
+  <si>
+    <t>state social benefits post mpc</t>
+  </si>
+  <si>
+    <t>$mpc09 [1] 0.245 0.105 0.056 0.056 0.056 0.056 0.056 0.056</t>
+  </si>
+  <si>
+    <t>rebate checks post mpc</t>
+  </si>
+  <si>
+    <t>$mpc07 [1] 0.140 0.100 0.100 0.050 0.050 0.050 0.050 0.050 0.050 0.030 0.030 0.030 0.025 0.020 0.015 0.010 0.005</t>
+  </si>
+  <si>
+    <t>rebate checks arp post mpc</t>
+  </si>
+  <si>
+    <t>$mpc02 [1] 0.20 0.17 0.16 0.15 0.09 0.05 0.05 0.04</t>
+  </si>
+  <si>
+    <t>federal ui post mpc</t>
+  </si>
+  <si>
+    <t>state ui post mpc</t>
+  </si>
+  <si>
+    <t>federal subsidies post mpc</t>
+  </si>
+  <si>
+    <t>$mpc08 [1] 0.040 0.040 0.017 0.017 0.017 0.017 0.017 0.017 0.017 0.017 0.017 0.017</t>
+  </si>
+  <si>
+    <t>federal aid to small businesses arp</t>
+  </si>
+  <si>
+    <t>federal other direct aid arp post mpc</t>
+  </si>
+  <si>
+    <t>federal other vulnerable arp post mpc</t>
+  </si>
+  <si>
+    <t>federal student loans post mpc</t>
+  </si>
+  <si>
+    <t>input from the forecast Excel sheet (w)</t>
+  </si>
+  <si>
+    <t>federal ui minus neutral</t>
+  </si>
+  <si>
+    <t>state ui minus neutral</t>
+  </si>
+  <si>
+    <t>federal subsidies minus neutral</t>
+  </si>
+  <si>
+    <t>federal social benefits minus neutral</t>
+  </si>
+  <si>
+    <t>state social benefits minus neutral</t>
+  </si>
+  <si>
+    <t>rebate checks minus neutral</t>
+  </si>
+  <si>
+    <t>rebate checks arp minus neutral</t>
+  </si>
+  <si>
+    <t>federal aid to small businesses arp minus neutral</t>
+  </si>
+  <si>
+    <t>federal other direct aid arp minus neutral</t>
+  </si>
+  <si>
+    <t>federal student loans minus neutral</t>
+  </si>
+  <si>
+    <t>federal other vulnerable arp minus neutral</t>
+  </si>
+  <si>
+    <t>federal social benefits</t>
+  </si>
+  <si>
+    <t>state social beneftis</t>
+  </si>
+  <si>
+    <t>rebate checks</t>
+  </si>
+  <si>
+    <t>federal ui</t>
+  </si>
+  <si>
+    <t>state ui</t>
+  </si>
+  <si>
+    <t>federal subsidies</t>
+  </si>
+  <si>
+    <t>federal aid to small businesses</t>
+  </si>
+  <si>
+    <t>federal other direct aid arp</t>
+  </si>
+  <si>
+    <t>federal other vulnerable arp</t>
+  </si>
+  <si>
+    <t>federal student loans</t>
+  </si>
+  <si>
+    <t>rebate checks arp</t>
+  </si>
+  <si>
+    <t>federal other vulnterable arp</t>
+  </si>
+  <si>
+    <t>state social benefits</t>
+  </si>
+  <si>
+    <t>federal non corporate taxes</t>
+  </si>
+  <si>
+    <t>state non corporate taxes</t>
+  </si>
+  <si>
+    <t>federal corporate taxes</t>
+  </si>
+  <si>
+    <t>state corporate taxes</t>
+  </si>
+  <si>
+    <t>supply side ira</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>The purpose of this spreadsheet is to track the various data columns that are inputted into the FIM and how they result in FIM output. It maps all FIM variables directly to outputs. This sheet was created by Lorae in June 2021 for the purposes of refactoring and simplifying the FIM code.</t>
+  </si>
+  <si>
+    <t>map series to analysis</t>
+  </si>
+  <si>
+    <t>A sheet initially used by Lorae to keep track of the various data columns used in steps of FIM analysis. It helped her uncover which data analysis steps were redundant/unneeded and which were crucial to producing the FIM output.</t>
+  </si>
+  <si>
+    <t>README</t>
+  </si>
+  <si>
+    <t>The sheet you're currently reading.</t>
+  </si>
+  <si>
+    <t>FIM summary Jun24</t>
+  </si>
+  <si>
+    <t>A sheet used to track every single operation used in the FIM from start to finish. Input, throughput and output are labelled with variables w (raw input from the "Forecast.xlsx" sheet), x (processed input), a (throughput in the "minus neutral" step), b (throughput in the "post mpc" step), y (contributions output), and z (aggregated contributions output). This sheet revealed that the "state subsidies" forecast was missing from our forecast sheet. It also enabled Lorae to fully refactor the code to produce a parallel FIM creating identical results with more modular steps.</t>
+  </si>
+  <si>
+    <t>FIM summary Jul 24</t>
+  </si>
+  <si>
+    <t>What will hopefully contain new ordering of the FIM</t>
+  </si>
+  <si>
+    <t>Purpose of this sheet</t>
+  </si>
+  <si>
+    <t>Table of contents</t>
+  </si>
+  <si>
+    <t>This column contains the actual inputs we have in the "forecast.xlsx" sheet for the FIM</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>These columns represent FIM output. Column y represents FIM contributions as disaggregated values. Column z represents the sums of column y terms that produce FIM top-line values that we publish online.</t>
+  </si>
+  <si>
+    <t>These columns track all the intermediate steps we use to produce FIM output! Column x shows how the medicare, medicaid grants, and medicaid variables are summed/differenced to produce federal health outlays and state health outlays. Then, we apply the minus neutral calculation on input (x) to produce throughput (a) : minus neutral values. After calculating minus neutrals, we apply the displayed MPC vectors to throughput (a) to produce the "post mpc" throughput (b). Then, we apply the contributions equations to the throughput results to produce output (y). Note that some series are produced directly using column (x), which you can because the throughput columns are mostly unpopulated.</t>
+  </si>
+  <si>
+    <t>INPUT/THROUGHPUT</t>
+  </si>
+  <si>
+    <t>THROUGPUT</t>
+  </si>
+  <si>
+    <t>OUTPUT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,8 +796,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,8 +824,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -510,11 +919,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -540,15 +958,53 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,6 +1013,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFF99CC"/>
+      <color rgb="FFFFCC99"/>
       <color rgb="FFFF6600"/>
     </mruColors>
   </colors>
@@ -833,28 +1292,275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA49EEA3-E40E-45F5-B449-6C1272590B27}">
+  <dimension ref="B2:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="7" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B7" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="C15:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B3:H5"/>
+    <mergeCell ref="C10:H14"/>
+    <mergeCell ref="C9:H9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="53" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" customWidth="1"/>
-    <col min="2" max="2" width="39.54296875" customWidth="1"/>
-    <col min="3" max="3" width="31.81640625" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" customWidth="1"/>
-    <col min="7" max="7" width="42.7265625" customWidth="1"/>
-    <col min="8" max="8" width="34.1796875" customWidth="1"/>
-    <col min="9" max="9" width="43.6328125" customWidth="1"/>
-    <col min="11" max="11" width="31.08984375" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" customWidth="1"/>
+    <col min="9" max="9" width="43.5703125" customWidth="1"/>
+    <col min="11" max="11" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -877,7 +1583,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -897,7 +1603,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -923,7 +1629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -945,7 +1651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -969,7 +1675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -993,7 +1699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +1724,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +1751,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1075,7 +1781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1105,7 +1811,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1126,7 +1832,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1168,7 +1874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1200,7 +1906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1230,7 +1936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1260,7 +1966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1290,7 +1996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1320,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1350,7 +2056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1377,7 +2083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1402,7 +2108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1437,7 +2143,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1469,7 +2175,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1501,7 +2207,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1529,7 +2235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>42</v>
       </c>
@@ -1554,7 +2260,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>44</v>
       </c>
@@ -1579,7 +2285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>45</v>
       </c>
@@ -1597,7 +2303,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>46</v>
       </c>
@@ -1614,14 +2320,14 @@
       <c r="G29" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="18" t="s">
         <v>9</v>
       </c>
       <c r="L29" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>47</v>
       </c>
@@ -1638,11 +2344,11 @@
       <c r="G30" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="K30" s="19" t="s">
+      <c r="K30" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>48</v>
       </c>
@@ -1663,7 +2369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>49</v>
       </c>
@@ -1681,7 +2387,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>50</v>
       </c>
@@ -1699,7 +2405,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>52</v>
       </c>
@@ -1710,7 +2416,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F35" s="17" t="s">
         <v>108</v>
       </c>
@@ -1718,27 +2424,25 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F36" s="8"/>
       <c r="G36" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="18"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F37" s="8"/>
       <c r="G37" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H37" s="18"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F38" s="10"/>
       <c r="G38" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F39" s="6" t="s">
         <v>94</v>
       </c>
@@ -1746,7 +2450,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F40" s="15" t="s">
         <v>102</v>
       </c>
@@ -1754,54 +2458,817 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F41" s="4"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F42" s="4"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F43" s="4"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F44" s="4"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F47" s="4"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F48" s="4"/>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F50" s="4"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F51" s="4"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G52" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7033BB19-1390-4BB5-AB4F-2126B7F80D39}">
+  <dimension ref="B2:V36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4" customWidth="1"/>
+    <col min="8" max="8" width="40.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="10" max="10" width="38" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" customWidth="1"/>
+    <col min="12" max="12" width="40.85546875" customWidth="1"/>
+    <col min="13" max="13" width="4" customWidth="1"/>
+    <col min="14" max="14" width="32.85546875" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="16" max="16" width="51.28515625" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" customWidth="1"/>
+    <col min="18" max="18" width="36.85546875" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" customWidth="1"/>
+    <col min="20" max="20" width="37.7109375" customWidth="1"/>
+    <col min="21" max="21" width="3.42578125" customWidth="1"/>
+    <col min="22" max="22" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="V3" s="20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="R4" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="35"/>
+    </row>
+    <row r="6" spans="2:22" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" t="s">
+        <v>116</v>
+      </c>
+      <c r="P7" t="s">
+        <v>118</v>
+      </c>
+      <c r="R7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="V7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>123</v>
+      </c>
+      <c r="P8" t="s">
+        <v>125</v>
+      </c>
+      <c r="R8" t="s">
+        <v>127</v>
+      </c>
+      <c r="T8" s="19"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" t="s">
+        <v>124</v>
+      </c>
+      <c r="P9" t="s">
+        <v>126</v>
+      </c>
+      <c r="R9" t="s">
+        <v>128</v>
+      </c>
+      <c r="T9" s="19"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="29"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" t="s">
+        <v>120</v>
+      </c>
+      <c r="P11" t="s">
+        <v>121</v>
+      </c>
+      <c r="R11" t="s">
+        <v>122</v>
+      </c>
+      <c r="T11" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="V11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="29"/>
+      <c r="T12" s="19"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="29"/>
+      <c r="T13" s="19"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="29"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J15" t="s">
+        <v>136</v>
+      </c>
+      <c r="L15" t="s">
+        <v>141</v>
+      </c>
+      <c r="N15" t="s">
+        <v>145</v>
+      </c>
+      <c r="P15" t="s">
+        <v>150</v>
+      </c>
+      <c r="R15" t="s">
+        <v>151</v>
+      </c>
+      <c r="T15" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="V15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>135</v>
+      </c>
+      <c r="J16" t="s">
+        <v>137</v>
+      </c>
+      <c r="L16" t="s">
+        <v>141</v>
+      </c>
+      <c r="N16" t="s">
+        <v>146</v>
+      </c>
+      <c r="P16" t="s">
+        <v>150</v>
+      </c>
+      <c r="R16" t="s">
+        <v>152</v>
+      </c>
+      <c r="T16" s="19"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" t="s">
+        <v>135</v>
+      </c>
+      <c r="J17" t="s">
+        <v>138</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="N17" t="s">
+        <v>147</v>
+      </c>
+      <c r="P17" t="s">
+        <v>150</v>
+      </c>
+      <c r="R17" t="s">
+        <v>153</v>
+      </c>
+      <c r="T17" s="19"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" t="s">
+        <v>135</v>
+      </c>
+      <c r="J18" t="s">
+        <v>139</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N18" t="s">
+        <v>148</v>
+      </c>
+      <c r="P18" t="s">
+        <v>150</v>
+      </c>
+      <c r="R18" t="s">
+        <v>154</v>
+      </c>
+      <c r="T18" s="19"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
+        <v>135</v>
+      </c>
+      <c r="J19" t="s">
+        <v>140</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="N19" t="s">
+        <v>149</v>
+      </c>
+      <c r="P19" t="s">
+        <v>150</v>
+      </c>
+      <c r="R19" t="s">
+        <v>155</v>
+      </c>
+      <c r="T19" s="19"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="29"/>
+    </row>
+    <row r="21" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="F21" t="s">
+        <v>202</v>
+      </c>
+      <c r="H21" t="s">
+        <v>135</v>
+      </c>
+      <c r="J21" t="s">
+        <v>194</v>
+      </c>
+      <c r="L21" t="s">
+        <v>163</v>
+      </c>
+      <c r="N21" t="s">
+        <v>175</v>
+      </c>
+      <c r="P21" t="s">
+        <v>150</v>
+      </c>
+      <c r="R21" t="s">
+        <v>81</v>
+      </c>
+      <c r="T21" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="V21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="F22" t="s">
+        <v>203</v>
+      </c>
+      <c r="H22" t="s">
+        <v>135</v>
+      </c>
+      <c r="J22" t="s">
+        <v>195</v>
+      </c>
+      <c r="L22" t="s">
+        <v>163</v>
+      </c>
+      <c r="N22" t="s">
+        <v>176</v>
+      </c>
+      <c r="P22" t="s">
+        <v>150</v>
+      </c>
+      <c r="R22" t="s">
+        <v>82</v>
+      </c>
+      <c r="T22" s="19"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" t="s">
+        <v>135</v>
+      </c>
+      <c r="J23" t="s">
+        <v>196</v>
+      </c>
+      <c r="L23" t="s">
+        <v>177</v>
+      </c>
+      <c r="N23" t="s">
+        <v>178</v>
+      </c>
+      <c r="P23" t="s">
+        <v>150</v>
+      </c>
+      <c r="R23" t="s">
+        <v>77</v>
+      </c>
+      <c r="T23" s="19"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="F24" t="s">
+        <v>212</v>
+      </c>
+      <c r="H24" t="s">
+        <v>135</v>
+      </c>
+      <c r="J24" t="s">
+        <v>197</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="N24" t="s">
+        <v>180</v>
+      </c>
+      <c r="P24" t="s">
+        <v>150</v>
+      </c>
+      <c r="R24" t="s">
+        <v>78</v>
+      </c>
+      <c r="T24" s="19"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="F25" t="s">
+        <v>205</v>
+      </c>
+      <c r="H25" t="s">
+        <v>135</v>
+      </c>
+      <c r="J25" t="s">
+        <v>191</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="N25" t="s">
+        <v>182</v>
+      </c>
+      <c r="P25" t="s">
+        <v>150</v>
+      </c>
+      <c r="R25" t="s">
+        <v>75</v>
+      </c>
+      <c r="T25" s="19"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" t="s">
+        <v>206</v>
+      </c>
+      <c r="H26" t="s">
+        <v>135</v>
+      </c>
+      <c r="J26" t="s">
+        <v>192</v>
+      </c>
+      <c r="L26" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="N26" t="s">
+        <v>183</v>
+      </c>
+      <c r="P26" t="s">
+        <v>150</v>
+      </c>
+      <c r="R26" t="s">
+        <v>76</v>
+      </c>
+      <c r="T26" s="19"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" t="s">
+        <v>207</v>
+      </c>
+      <c r="H27" t="s">
+        <v>135</v>
+      </c>
+      <c r="J27" t="s">
+        <v>193</v>
+      </c>
+      <c r="L27" t="s">
+        <v>162</v>
+      </c>
+      <c r="N27" t="s">
+        <v>184</v>
+      </c>
+      <c r="P27" t="s">
+        <v>150</v>
+      </c>
+      <c r="R27" t="s">
+        <v>73</v>
+      </c>
+      <c r="T27" s="19"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="F28" t="s">
+        <v>208</v>
+      </c>
+      <c r="H28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J28" t="s">
+        <v>198</v>
+      </c>
+      <c r="L28" t="s">
+        <v>185</v>
+      </c>
+      <c r="N28" t="s">
+        <v>186</v>
+      </c>
+      <c r="P28" t="s">
+        <v>150</v>
+      </c>
+      <c r="R28" t="s">
+        <v>74</v>
+      </c>
+      <c r="T28" s="19"/>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="F29" t="s">
+        <v>209</v>
+      </c>
+      <c r="H29" t="s">
+        <v>135</v>
+      </c>
+      <c r="J29" t="s">
+        <v>199</v>
+      </c>
+      <c r="L29" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="N29" t="s">
+        <v>187</v>
+      </c>
+      <c r="P29" t="s">
+        <v>150</v>
+      </c>
+      <c r="R29" t="s">
+        <v>80</v>
+      </c>
+      <c r="T29" s="19"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="F30" t="s">
+        <v>210</v>
+      </c>
+      <c r="H30" t="s">
+        <v>135</v>
+      </c>
+      <c r="J30" t="s">
+        <v>201</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="N30" t="s">
+        <v>188</v>
+      </c>
+      <c r="P30" t="s">
+        <v>150</v>
+      </c>
+      <c r="R30" t="s">
+        <v>79</v>
+      </c>
+      <c r="T30" s="19"/>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="F31" t="s">
+        <v>211</v>
+      </c>
+      <c r="H31" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" t="s">
+        <v>200</v>
+      </c>
+      <c r="L31" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="N31" t="s">
+        <v>189</v>
+      </c>
+      <c r="P31" t="s">
+        <v>150</v>
+      </c>
+      <c r="R31" t="s">
+        <v>87</v>
+      </c>
+      <c r="T31" s="19"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" s="23"/>
+      <c r="H32" t="s">
+        <v>135</v>
+      </c>
+      <c r="J32" t="s">
+        <v>159</v>
+      </c>
+      <c r="L32" t="s">
+        <v>162</v>
+      </c>
+      <c r="N32" t="s">
+        <v>164</v>
+      </c>
+      <c r="P32" t="s">
+        <v>150</v>
+      </c>
+      <c r="R32" t="s">
+        <v>95</v>
+      </c>
+      <c r="T32" s="19"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" t="s">
+        <v>169</v>
+      </c>
+      <c r="H33" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" t="s">
+        <v>160</v>
+      </c>
+      <c r="L33" t="s">
+        <v>163</v>
+      </c>
+      <c r="N33" t="s">
+        <v>165</v>
+      </c>
+      <c r="P33" t="s">
+        <v>150</v>
+      </c>
+      <c r="R33" t="s">
+        <v>97</v>
+      </c>
+      <c r="T33" s="19"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="19"/>
+      <c r="T34" s="19"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F35" t="s">
+        <v>172</v>
+      </c>
+      <c r="H35" t="s">
+        <v>135</v>
+      </c>
+      <c r="J35" t="s">
+        <v>161</v>
+      </c>
+      <c r="L35" t="s">
+        <v>163</v>
+      </c>
+      <c r="N35" t="s">
+        <v>166</v>
+      </c>
+      <c r="P35" t="s">
+        <v>150</v>
+      </c>
+      <c r="R35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="29"/>
+      <c r="D36" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D4:P4"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="T11:T13"/>
+    <mergeCell ref="T15:T19"/>
+    <mergeCell ref="T21:T34"/>
+    <mergeCell ref="D33:D34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docs: improve formatting in variables tracker sheet
</commit_message>
<xml_diff>
--- a/docs/variables_tracker.xlsx
+++ b/docs/variables_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\FIM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD810A0-43DE-4347-B4A6-8669173481BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524BBC2C-BA76-47F5-95C2-30E9CEC03528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3390" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="239">
   <si>
     <t>Step 1: Input</t>
   </si>
@@ -474,9 +474,6 @@
   </si>
   <si>
     <t>supply side ira post mpc</t>
-  </si>
-  <si>
-    <t>state corporate taxes post mpc</t>
   </si>
   <si>
     <t>y = 400*b / lag(gdp)</t>
@@ -932,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -966,45 +963,38 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1305,224 +1295,224 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="7" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B7" s="27" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="7" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="30" t="s">
-        <v>232</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="C15" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2514,8 +2504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7033BB19-1390-4BB5-AB4F-2126B7F80D39}">
   <dimension ref="B2:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="H3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,97 +2535,97 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="26" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="V3" s="19" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="R4" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="R3" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="V3" s="20" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>236</v>
-      </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="R4" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="35"/>
-    </row>
-    <row r="6" spans="2:22" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34" t="s">
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+    </row>
+    <row r="6" spans="2:22" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34" t="s">
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34" t="s">
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" t="s">
         <v>116</v>
       </c>
       <c r="F7" t="s">
@@ -2647,7 +2637,7 @@
       <c r="R7" t="s">
         <v>119</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="T7" s="30" t="s">
         <v>131</v>
       </c>
       <c r="V7" t="s">
@@ -2655,7 +2645,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" t="s">
         <v>123</v>
       </c>
       <c r="F8" t="s">
@@ -2667,10 +2657,10 @@
       <c r="R8" t="s">
         <v>127</v>
       </c>
-      <c r="T8" s="19"/>
+      <c r="T8" s="30"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" t="s">
         <v>124</v>
       </c>
       <c r="F9" t="s">
@@ -2682,13 +2672,10 @@
       <c r="R9" t="s">
         <v>128</v>
       </c>
-      <c r="T9" s="19"/>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
+      <c r="T9" s="30"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="B11" t="s">
         <v>120</v>
       </c>
       <c r="F11" t="s">
@@ -2700,7 +2687,7 @@
       <c r="R11" t="s">
         <v>122</v>
       </c>
-      <c r="T11" s="19" t="s">
+      <c r="T11" s="30" t="s">
         <v>132</v>
       </c>
       <c r="V11" t="s">
@@ -2708,19 +2695,14 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="29"/>
-      <c r="T12" s="19"/>
+      <c r="T12" s="30"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="29"/>
-      <c r="T13" s="19"/>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="29"/>
+      <c r="T13" s="30"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
-        <v>215</v>
+      <c r="B15" t="s">
+        <v>214</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
@@ -2738,21 +2720,21 @@
         <v>145</v>
       </c>
       <c r="P15" t="s">
+        <v>149</v>
+      </c>
+      <c r="R15" t="s">
         <v>150</v>
       </c>
-      <c r="R15" t="s">
-        <v>151</v>
-      </c>
-      <c r="T15" s="19" t="s">
-        <v>156</v>
+      <c r="T15" s="30" t="s">
+        <v>155</v>
       </c>
       <c r="V15" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
-        <v>216</v>
+      <c r="B16" t="s">
+        <v>215</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -2770,16 +2752,16 @@
         <v>146</v>
       </c>
       <c r="P16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R16" t="s">
-        <v>152</v>
-      </c>
-      <c r="T16" s="19"/>
+        <v>151</v>
+      </c>
+      <c r="T16" s="30"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
-        <v>217</v>
+      <c r="B17" t="s">
+        <v>216</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -2790,23 +2772,23 @@
       <c r="J17" t="s">
         <v>138</v>
       </c>
-      <c r="L17" s="22" t="s">
+      <c r="L17" t="s">
         <v>142</v>
       </c>
       <c r="N17" t="s">
         <v>147</v>
       </c>
       <c r="P17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R17" t="s">
-        <v>153</v>
-      </c>
-      <c r="T17" s="19"/>
+        <v>152</v>
+      </c>
+      <c r="T17" s="30"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
-        <v>219</v>
+      <c r="B18" t="s">
+        <v>218</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
@@ -2824,16 +2806,16 @@
         <v>148</v>
       </c>
       <c r="P18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R18" t="s">
-        <v>154</v>
-      </c>
-      <c r="T18" s="19"/>
+        <v>153</v>
+      </c>
+      <c r="T18" s="30"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
-        <v>218</v>
+      <c r="B19" t="s">
+        <v>217</v>
       </c>
       <c r="F19" t="s">
         <v>21</v>
@@ -2844,419 +2826,415 @@
       <c r="J19" t="s">
         <v>140</v>
       </c>
-      <c r="L19" s="22" t="s">
+      <c r="L19" t="s">
         <v>142</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19">
+        <v>400</v>
+      </c>
+      <c r="P19" t="s">
         <v>149</v>
       </c>
-      <c r="P19" t="s">
-        <v>150</v>
-      </c>
       <c r="R19" t="s">
-        <v>155</v>
-      </c>
-      <c r="T19" s="19"/>
-    </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="29"/>
+        <v>154</v>
+      </c>
+      <c r="T19" s="30"/>
     </row>
     <row r="21" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
-        <v>202</v>
+      <c r="B21" t="s">
+        <v>201</v>
       </c>
       <c r="F21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H21" t="s">
         <v>135</v>
       </c>
       <c r="J21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R21" t="s">
         <v>81</v>
       </c>
-      <c r="T21" s="19" t="s">
-        <v>158</v>
+      <c r="T21" s="30" t="s">
+        <v>157</v>
       </c>
       <c r="V21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
-        <v>214</v>
+      <c r="B22" t="s">
+        <v>213</v>
       </c>
       <c r="F22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H22" t="s">
         <v>135</v>
       </c>
       <c r="J22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R22" t="s">
         <v>82</v>
       </c>
-      <c r="T22" s="19"/>
+      <c r="T22" s="30"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
-        <v>204</v>
+      <c r="B23" t="s">
+        <v>203</v>
       </c>
       <c r="F23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H23" t="s">
         <v>135</v>
       </c>
       <c r="J23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L23" t="s">
+        <v>176</v>
+      </c>
+      <c r="N23" t="s">
         <v>177</v>
       </c>
-      <c r="N23" t="s">
-        <v>178</v>
-      </c>
       <c r="P23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R23" t="s">
         <v>77</v>
       </c>
-      <c r="T23" s="19"/>
+      <c r="T23" s="30"/>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
-        <v>212</v>
+      <c r="B24" t="s">
+        <v>211</v>
       </c>
       <c r="F24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H24" t="s">
         <v>135</v>
       </c>
       <c r="J24" t="s">
-        <v>197</v>
-      </c>
-      <c r="L24" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="L24" t="s">
+        <v>178</v>
+      </c>
+      <c r="N24" t="s">
         <v>179</v>
       </c>
-      <c r="N24" t="s">
-        <v>180</v>
-      </c>
       <c r="P24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R24" t="s">
         <v>78</v>
       </c>
-      <c r="T24" s="19"/>
+      <c r="T24" s="30"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
-        <v>205</v>
+      <c r="B25" t="s">
+        <v>204</v>
       </c>
       <c r="F25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H25" t="s">
         <v>135</v>
       </c>
       <c r="J25" t="s">
-        <v>191</v>
-      </c>
-      <c r="L25" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L25" t="s">
+        <v>180</v>
+      </c>
+      <c r="N25" t="s">
         <v>181</v>
       </c>
-      <c r="N25" t="s">
-        <v>182</v>
-      </c>
       <c r="P25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R25" t="s">
         <v>75</v>
       </c>
-      <c r="T25" s="19"/>
+      <c r="T25" s="30"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
-        <v>206</v>
+      <c r="B26" t="s">
+        <v>205</v>
       </c>
       <c r="F26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H26" t="s">
         <v>135</v>
       </c>
       <c r="J26" t="s">
-        <v>192</v>
-      </c>
-      <c r="L26" s="22" t="s">
-        <v>181</v>
+        <v>191</v>
+      </c>
+      <c r="L26" t="s">
+        <v>180</v>
       </c>
       <c r="N26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R26" t="s">
         <v>76</v>
       </c>
-      <c r="T26" s="19"/>
+      <c r="T26" s="30"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B27" s="29" t="s">
-        <v>207</v>
+      <c r="B27" t="s">
+        <v>206</v>
       </c>
       <c r="F27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H27" t="s">
         <v>135</v>
       </c>
       <c r="J27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R27" t="s">
         <v>73</v>
       </c>
-      <c r="T27" s="19"/>
+      <c r="T27" s="30"/>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
-        <v>208</v>
+      <c r="B28" t="s">
+        <v>207</v>
       </c>
       <c r="F28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H28" t="s">
         <v>135</v>
       </c>
       <c r="J28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L28" t="s">
+        <v>184</v>
+      </c>
+      <c r="N28" t="s">
         <v>185</v>
       </c>
-      <c r="N28" t="s">
-        <v>186</v>
-      </c>
       <c r="P28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R28" t="s">
         <v>74</v>
       </c>
-      <c r="T28" s="19"/>
+      <c r="T28" s="30"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
-        <v>209</v>
+      <c r="B29" t="s">
+        <v>208</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H29" t="s">
         <v>135</v>
       </c>
       <c r="J29" t="s">
-        <v>199</v>
-      </c>
-      <c r="L29" s="22" t="s">
-        <v>179</v>
+        <v>198</v>
+      </c>
+      <c r="L29" t="s">
+        <v>178</v>
       </c>
       <c r="N29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R29" t="s">
         <v>80</v>
       </c>
-      <c r="T29" s="19"/>
+      <c r="T29" s="30"/>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
-        <v>213</v>
+      <c r="B30" t="s">
+        <v>212</v>
       </c>
       <c r="F30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H30" t="s">
         <v>135</v>
       </c>
       <c r="J30" t="s">
-        <v>201</v>
-      </c>
-      <c r="L30" s="22" t="s">
-        <v>181</v>
+        <v>200</v>
+      </c>
+      <c r="L30" t="s">
+        <v>180</v>
       </c>
       <c r="N30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R30" t="s">
         <v>79</v>
       </c>
-      <c r="T30" s="19"/>
+      <c r="T30" s="30"/>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
-        <v>211</v>
+      <c r="B31" t="s">
+        <v>210</v>
       </c>
       <c r="F31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H31" t="s">
         <v>135</v>
       </c>
       <c r="J31" t="s">
-        <v>200</v>
-      </c>
-      <c r="L31" s="22" t="s">
-        <v>181</v>
+        <v>199</v>
+      </c>
+      <c r="L31" t="s">
+        <v>180</v>
       </c>
       <c r="N31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R31" t="s">
         <v>87</v>
       </c>
-      <c r="T31" s="19"/>
+      <c r="T31" s="30"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="F32" s="23"/>
+      <c r="B32" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="F32" s="21"/>
       <c r="H32" t="s">
         <v>135</v>
       </c>
       <c r="J32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R32" t="s">
         <v>95</v>
       </c>
-      <c r="T32" s="19"/>
+      <c r="T32" s="30"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
+      <c r="B33" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>170</v>
+      <c r="D33" s="30" t="s">
+        <v>169</v>
       </c>
       <c r="F33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H33" t="s">
         <v>135</v>
       </c>
       <c r="J33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R33" t="s">
         <v>97</v>
       </c>
-      <c r="T33" s="19"/>
+      <c r="T33" s="30"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="29" t="s">
+      <c r="B34" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34" s="30"/>
+      <c r="T34" s="30"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" t="s">
         <v>171</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="T34" s="19"/>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="F35" t="s">
-        <v>172</v>
       </c>
       <c r="H35" t="s">
         <v>135</v>
       </c>
       <c r="J35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R35" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="29"/>
-      <c r="D36" s="19"/>
+      <c r="D36" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>